<commit_message>
filled out full NQBH's ROMSOC timesheet
</commit_message>
<xml_diff>
--- a/timesheet/H2020_time_sheet_2021_WIAS_MSCA_ROMSOC_Nguyen.xlsx
+++ b/timesheet/H2020_time_sheet_2021_WIAS_MSCA_ROMSOC_Nguyen.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="60">
   <si>
     <t xml:space="preserve">Person working on the action:</t>
   </si>
@@ -293,7 +293,7 @@
     <numFmt numFmtId="171" formatCode="ddd"/>
     <numFmt numFmtId="172" formatCode="@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -390,6 +390,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -603,7 +608,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -936,6 +941,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="172" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -960,7 +969,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2542,7 +2551,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH8" activeCellId="0" sqref="AH8"/>
+      <selection pane="topLeft" activeCell="AH7" activeCellId="0" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4509,7 +4518,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="AH7" activeCellId="0" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4918,42 +4927,86 @@
       <c r="A7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="C7" s="31"/>
       <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
+      <c r="E7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="H7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="I7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
+      <c r="L7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="M7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="N7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="O7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="P7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="Q7" s="31"/>
       <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
+      <c r="S7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="T7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="U7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="V7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="W7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="X7" s="31"/>
       <c r="Y7" s="31"/>
-      <c r="Z7" s="31"/>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
-      <c r="AD7" s="31"/>
+      <c r="Z7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AE7" s="31"/>
       <c r="AF7" s="32"/>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34"/>
+        <v>168</v>
+      </c>
+      <c r="AH7" s="83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
@@ -5001,7 +5054,7 @@
       </c>
       <c r="B9" s="39" t="n">
         <f aca="false">SUM(B7:B8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="39" t="n">
         <f aca="false">SUM(C7:C8)</f>
@@ -5013,23 +5066,23 @@
       </c>
       <c r="E9" s="39" t="n">
         <f aca="false">SUM(E7:E8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F9" s="39" t="n">
         <f aca="false">SUM(F7:F8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9" s="39" t="n">
         <f aca="false">SUM(G7:G8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H9" s="39" t="n">
         <f aca="false">SUM(H7:H8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9" s="39" t="n">
         <f aca="false">SUM(I7:I8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="39" t="n">
         <f aca="false">SUM(J7:J8)</f>
@@ -5041,23 +5094,23 @@
       </c>
       <c r="L9" s="39" t="n">
         <f aca="false">SUM(L7:L8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M9" s="39" t="n">
         <f aca="false">SUM(M7:M8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N9" s="39" t="n">
         <f aca="false">SUM(N7:N8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O9" s="39" t="n">
         <f aca="false">SUM(O7:O8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P9" s="39" t="n">
         <f aca="false">SUM(P7:P8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="39" t="n">
         <f aca="false">SUM(Q7:Q8)</f>
@@ -5069,23 +5122,23 @@
       </c>
       <c r="S9" s="39" t="n">
         <f aca="false">SUM(S7:S8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T9" s="39" t="n">
         <f aca="false">SUM(T7:T8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U9" s="39" t="n">
         <f aca="false">SUM(U7:U8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V9" s="39" t="n">
         <f aca="false">SUM(V7:V8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W9" s="39" t="n">
         <f aca="false">SUM(W7:W8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X9" s="39" t="n">
         <f aca="false">SUM(X7:X8)</f>
@@ -5097,23 +5150,23 @@
       </c>
       <c r="Z9" s="39" t="n">
         <f aca="false">SUM(Z7:Z8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA9" s="39" t="n">
         <f aca="false">SUM(AA7:AA8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB9" s="39" t="n">
         <f aca="false">SUM(AB7:AB8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC9" s="39" t="n">
         <f aca="false">SUM(AC7:AC8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD9" s="39" t="n">
         <f aca="false">SUM(AD7:AD8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE9" s="39" t="n">
         <f aca="false">SUM(AE7:AE8)</f>
@@ -5125,7 +5178,7 @@
       </c>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -5682,7 +5735,7 @@
       </c>
       <c r="B19" s="52" t="n">
         <f aca="false">B9+B13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="52" t="n">
         <f aca="false">C9+C13</f>
@@ -5694,23 +5747,23 @@
       </c>
       <c r="E19" s="52" t="n">
         <f aca="false">E9+E13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F19" s="52" t="n">
         <f aca="false">F9+F13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G19" s="52" t="n">
         <f aca="false">G9+G13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H19" s="52" t="n">
         <f aca="false">H9+H13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I19" s="52" t="n">
         <f aca="false">I9+I13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J19" s="52" t="n">
         <f aca="false">J9+J13</f>
@@ -5722,23 +5775,23 @@
       </c>
       <c r="L19" s="52" t="n">
         <f aca="false">L9+L13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M19" s="52" t="n">
         <f aca="false">M9+M13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N19" s="52" t="n">
         <f aca="false">N9+N13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O19" s="52" t="n">
         <f aca="false">O9+O13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P19" s="52" t="n">
         <f aca="false">P9+P13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="52" t="n">
         <f aca="false">Q9+Q13</f>
@@ -5750,23 +5803,23 @@
       </c>
       <c r="S19" s="52" t="n">
         <f aca="false">S9+S13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T19" s="52" t="n">
         <f aca="false">T9+T13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U19" s="52" t="n">
         <f aca="false">U9+U13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V19" s="52" t="n">
         <f aca="false">V9+V13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W19" s="52" t="n">
         <f aca="false">W9+W13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X19" s="52" t="n">
         <f aca="false">X9+X13</f>
@@ -5778,23 +5831,23 @@
       </c>
       <c r="Z19" s="52" t="n">
         <f aca="false">Z9+Z13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA19" s="52" t="n">
         <f aca="false">AA9+AA13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB19" s="52" t="n">
         <f aca="false">AB9+AB13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC19" s="52" t="n">
         <f aca="false">AC9+AC13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD19" s="52" t="n">
         <f aca="false">AD9+AD13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE19" s="52" t="n">
         <f aca="false">AE9+AE13</f>
@@ -5806,7 +5859,7 @@
       </c>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="AH19" s="54"/>
     </row>
@@ -5847,7 +5900,7 @@
       <c r="AF20" s="56"/>
       <c r="AG20" s="57" t="n">
         <f aca="false">AG18+AG19</f>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="AH20" s="58"/>
     </row>
@@ -6433,7 +6486,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="AH7" activeCellId="0" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6838,42 +6891,88 @@
       <c r="A7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="B7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
+      <c r="I7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="L7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="M7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="N7" s="31"/>
       <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
+      <c r="P7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="S7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="T7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="U7" s="31"/>
       <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="31"/>
-      <c r="Z7" s="31"/>
-      <c r="AA7" s="31"/>
+      <c r="W7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="X7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AB7" s="31"/>
       <c r="AC7" s="31"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="31"/>
+      <c r="AD7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AF7" s="32"/>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34"/>
+        <v>176</v>
+      </c>
+      <c r="AH7" s="83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
@@ -6921,23 +7020,23 @@
       </c>
       <c r="B9" s="39" t="n">
         <f aca="false">SUM(B7:B8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="39" t="n">
         <f aca="false">SUM(C7:C8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9" s="39" t="n">
         <f aca="false">SUM(D7:D8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="39" t="n">
         <f aca="false">SUM(E7:E8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F9" s="39" t="n">
         <f aca="false">SUM(F7:F8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9" s="39" t="n">
         <f aca="false">SUM(G7:G8)</f>
@@ -6949,23 +7048,23 @@
       </c>
       <c r="I9" s="39" t="n">
         <f aca="false">SUM(I7:I8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="39" t="n">
         <f aca="false">SUM(J7:J8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K9" s="39" t="n">
         <f aca="false">SUM(K7:K8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L9" s="39" t="n">
         <f aca="false">SUM(L7:L8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M9" s="39" t="n">
         <f aca="false">SUM(M7:M8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N9" s="39" t="n">
         <f aca="false">SUM(N7:N8)</f>
@@ -6977,23 +7076,23 @@
       </c>
       <c r="P9" s="39" t="n">
         <f aca="false">SUM(P7:P8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="39" t="n">
         <f aca="false">SUM(Q7:Q8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R9" s="39" t="n">
         <f aca="false">SUM(R7:R8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S9" s="39" t="n">
         <f aca="false">SUM(S7:S8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T9" s="39" t="n">
         <f aca="false">SUM(T7:T8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U9" s="39" t="n">
         <f aca="false">SUM(U7:U8)</f>
@@ -7005,23 +7104,23 @@
       </c>
       <c r="W9" s="39" t="n">
         <f aca="false">SUM(W7:W8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X9" s="39" t="n">
         <f aca="false">SUM(X7:X8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y9" s="39" t="n">
         <f aca="false">SUM(Y7:Y8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z9" s="39" t="n">
         <f aca="false">SUM(Z7:Z8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA9" s="39" t="n">
         <f aca="false">SUM(AA7:AA8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB9" s="39" t="n">
         <f aca="false">SUM(AB7:AB8)</f>
@@ -7033,16 +7132,16 @@
       </c>
       <c r="AD9" s="39" t="n">
         <f aca="false">SUM(AD7:AD8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE9" s="39" t="n">
         <f aca="false">SUM(AE7:AE8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF9" s="39"/>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -7593,23 +7692,23 @@
       </c>
       <c r="B19" s="52" t="n">
         <f aca="false">B9+B13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="52" t="n">
         <f aca="false">C9+C13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D19" s="52" t="n">
         <f aca="false">D9+D13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E19" s="52" t="n">
         <f aca="false">E9+E13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F19" s="52" t="n">
         <f aca="false">F9+F13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G19" s="52" t="n">
         <f aca="false">G9+G13</f>
@@ -7621,23 +7720,23 @@
       </c>
       <c r="I19" s="52" t="n">
         <f aca="false">I9+I13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J19" s="52" t="n">
         <f aca="false">J9+J13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K19" s="52" t="n">
         <f aca="false">K9+K13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L19" s="52" t="n">
         <f aca="false">L9+L13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M19" s="52" t="n">
         <f aca="false">M9+M13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N19" s="52" t="n">
         <f aca="false">N9+N13</f>
@@ -7649,23 +7748,23 @@
       </c>
       <c r="P19" s="52" t="n">
         <f aca="false">P9+P13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="52" t="n">
         <f aca="false">Q9+Q13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R19" s="52" t="n">
         <f aca="false">R9+R13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S19" s="52" t="n">
         <f aca="false">S9+S13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T19" s="52" t="n">
         <f aca="false">T9+T13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U19" s="52" t="n">
         <f aca="false">U9+U13</f>
@@ -7677,23 +7776,23 @@
       </c>
       <c r="W19" s="52" t="n">
         <f aca="false">W9+W13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X19" s="52" t="n">
         <f aca="false">X9+X13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y19" s="52" t="n">
         <f aca="false">Y9+Y13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z19" s="52" t="n">
         <f aca="false">Z9+Z13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA19" s="52" t="n">
         <f aca="false">AA9+AA13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB19" s="52" t="n">
         <f aca="false">AB9+AB13</f>
@@ -7705,16 +7804,16 @@
       </c>
       <c r="AD19" s="52" t="n">
         <f aca="false">AD9+AD13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE19" s="52" t="n">
         <f aca="false">AE9+AE13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF19" s="52"/>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH19" s="54"/>
     </row>
@@ -7755,7 +7854,7 @@
       <c r="AF20" s="56"/>
       <c r="AG20" s="57" t="n">
         <f aca="false">AG18+AG19</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH20" s="58"/>
     </row>
@@ -8341,7 +8440,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="X8" activeCellId="0" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8750,42 +8849,86 @@
       <c r="A7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
+      <c r="B7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
+      <c r="G7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="H7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="I7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="L7" s="31"/>
       <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
+      <c r="N7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="O7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="P7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="S7" s="31"/>
       <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
+      <c r="U7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="V7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="W7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="X7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="Y7" s="30"/>
       <c r="Z7" s="30"/>
       <c r="AA7" s="30"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="31"/>
-      <c r="AF7" s="87"/>
+      <c r="AB7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AF7" s="88"/>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34"/>
+        <v>168</v>
+      </c>
+      <c r="AH7" s="83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
@@ -8819,7 +8962,7 @@
       <c r="AC8" s="31"/>
       <c r="AD8" s="31"/>
       <c r="AE8" s="31"/>
-      <c r="AF8" s="87"/>
+      <c r="AF8" s="88"/>
       <c r="AG8" s="33" t="n">
         <f aca="false">SUM(B8:AF8)</f>
         <v>0</v>
@@ -8833,15 +8976,15 @@
       </c>
       <c r="B9" s="39" t="n">
         <f aca="false">SUM(B7:B8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="39" t="n">
         <f aca="false">SUM(C7:C8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9" s="39" t="n">
         <f aca="false">SUM(D7:D8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="39" t="n">
         <f aca="false">SUM(E7:E8)</f>
@@ -8853,23 +8996,23 @@
       </c>
       <c r="G9" s="39" t="n">
         <f aca="false">SUM(G7:G8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H9" s="39" t="n">
         <f aca="false">SUM(H7:H8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9" s="39" t="n">
         <f aca="false">SUM(I7:I8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="39" t="n">
         <f aca="false">SUM(J7:J8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K9" s="39" t="n">
         <f aca="false">SUM(K7:K8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L9" s="39" t="n">
         <f aca="false">SUM(L7:L8)</f>
@@ -8881,23 +9024,23 @@
       </c>
       <c r="N9" s="39" t="n">
         <f aca="false">SUM(N7:N8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O9" s="39" t="n">
         <f aca="false">SUM(O7:O8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P9" s="39" t="n">
         <f aca="false">SUM(P7:P8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="39" t="n">
         <f aca="false">SUM(Q7:Q8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R9" s="39" t="n">
         <f aca="false">SUM(R7:R8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S9" s="39" t="n">
         <f aca="false">SUM(S7:S8)</f>
@@ -8909,19 +9052,19 @@
       </c>
       <c r="U9" s="39" t="n">
         <f aca="false">SUM(U7:U8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V9" s="39" t="n">
         <f aca="false">SUM(V7:V8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W9" s="39" t="n">
         <f aca="false">SUM(W7:W8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X9" s="39" t="n">
         <f aca="false">SUM(X7:X8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y9" s="38" t="n">
         <f aca="false">SUM(Y7:Y8)</f>
@@ -8937,19 +9080,19 @@
       </c>
       <c r="AB9" s="39" t="n">
         <f aca="false">SUM(AB7:AB8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC9" s="39" t="n">
         <f aca="false">SUM(AC7:AC8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD9" s="39" t="n">
         <f aca="false">SUM(AD7:AD8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE9" s="39" t="n">
         <f aca="false">SUM(AE7:AE8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF9" s="38" t="n">
         <f aca="false">SUM(AF7:AF8)</f>
@@ -8957,7 +9100,7 @@
       </c>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -9033,7 +9176,7 @@
       <c r="AC11" s="31"/>
       <c r="AD11" s="31"/>
       <c r="AE11" s="31"/>
-      <c r="AF11" s="87"/>
+      <c r="AF11" s="88"/>
       <c r="AG11" s="33" t="n">
         <f aca="false">SUM(B11:AF11)</f>
         <v>0</v>
@@ -9072,7 +9215,7 @@
       <c r="AC12" s="31"/>
       <c r="AD12" s="31"/>
       <c r="AE12" s="31"/>
-      <c r="AF12" s="87"/>
+      <c r="AF12" s="88"/>
       <c r="AG12" s="33" t="n">
         <f aca="false">SUM(B12:AF12)</f>
         <v>0</v>
@@ -9285,7 +9428,7 @@
       <c r="AC15" s="31"/>
       <c r="AD15" s="31"/>
       <c r="AE15" s="31"/>
-      <c r="AF15" s="87"/>
+      <c r="AF15" s="88"/>
       <c r="AG15" s="43" t="n">
         <f aca="false">SUM(B15:AF15)</f>
         <v>0</v>
@@ -9326,7 +9469,7 @@
       <c r="AC16" s="31"/>
       <c r="AD16" s="31"/>
       <c r="AE16" s="31"/>
-      <c r="AF16" s="87"/>
+      <c r="AF16" s="88"/>
       <c r="AG16" s="43" t="n">
         <f aca="false">SUM(B16:AF16)</f>
         <v>0</v>
@@ -9367,7 +9510,7 @@
       <c r="AC17" s="31"/>
       <c r="AD17" s="31"/>
       <c r="AE17" s="31"/>
-      <c r="AF17" s="87"/>
+      <c r="AF17" s="88"/>
       <c r="AG17" s="43" t="n">
         <f aca="false">SUM(B17:AF17)</f>
         <v>0</v>
@@ -9514,15 +9657,15 @@
       </c>
       <c r="B19" s="52" t="n">
         <f aca="false">B9+B13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="52" t="n">
         <f aca="false">C9+C13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D19" s="52" t="n">
         <f aca="false">D9+D13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E19" s="52" t="n">
         <f aca="false">E9+E13</f>
@@ -9534,23 +9677,23 @@
       </c>
       <c r="G19" s="52" t="n">
         <f aca="false">G9+G13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H19" s="52" t="n">
         <f aca="false">H9+H13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I19" s="52" t="n">
         <f aca="false">I9+I13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J19" s="52" t="n">
         <f aca="false">J9+J13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K19" s="52" t="n">
         <f aca="false">K9+K13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L19" s="52" t="n">
         <f aca="false">L9+L13</f>
@@ -9562,23 +9705,23 @@
       </c>
       <c r="N19" s="52" t="n">
         <f aca="false">N9+N13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O19" s="52" t="n">
         <f aca="false">O9+O13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P19" s="52" t="n">
         <f aca="false">P9+P13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="52" t="n">
         <f aca="false">Q9+Q13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R19" s="52" t="n">
         <f aca="false">R9+R13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S19" s="52" t="n">
         <f aca="false">S9+S13</f>
@@ -9590,19 +9733,19 @@
       </c>
       <c r="U19" s="52" t="n">
         <f aca="false">U9+U13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V19" s="52" t="n">
         <f aca="false">V9+V13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W19" s="52" t="n">
         <f aca="false">W9+W13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X19" s="52" t="n">
         <f aca="false">X9+X13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y19" s="51" t="n">
         <f aca="false">Y9+Y13</f>
@@ -9618,19 +9761,19 @@
       </c>
       <c r="AB19" s="52" t="n">
         <f aca="false">AB9+AB13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC19" s="52" t="n">
         <f aca="false">AC9+AC13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD19" s="52" t="n">
         <f aca="false">AD9+AD13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE19" s="52" t="n">
         <f aca="false">AE9+AE13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF19" s="51" t="n">
         <f aca="false">AF9+AF13</f>
@@ -9638,7 +9781,7 @@
       </c>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="AH19" s="54"/>
     </row>
@@ -9679,7 +9822,7 @@
       <c r="AF20" s="56"/>
       <c r="AG20" s="57" t="n">
         <f aca="false">AG18+AG19</f>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="AH20" s="58"/>
     </row>
@@ -10265,28 +10408,28 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="89" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="89" t="s">
         <v>43</v>
       </c>
     </row>
@@ -10294,7 +10437,7 @@
       <c r="A3" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="89" t="s">
         <v>12</v>
       </c>
     </row>
@@ -10302,7 +10445,7 @@
       <c r="A4" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="89" t="s">
         <v>46</v>
       </c>
     </row>
@@ -10310,7 +10453,7 @@
       <c r="A5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="89" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10318,7 +10461,7 @@
       <c r="A6" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="C6" s="89" t="s">
         <v>50</v>
       </c>
     </row>
@@ -10346,34 +10489,34 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="90" t="s">
+      <c r="C13" s="91" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="90" t="n">
+      <c r="C14" s="91" t="n">
         <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="90" t="n">
+      <c r="C15" s="91" t="n">
         <v>765374</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="91" t="n">
+      <c r="C17" s="92" t="n">
         <v>2021</v>
       </c>
     </row>
@@ -12315,7 +12458,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH8" activeCellId="0" sqref="AH8"/>
+      <selection pane="topLeft" activeCell="AA17" activeCellId="0" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12763,46 +12906,26 @@
       <c r="Q7" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="R7" s="31" t="n">
-        <v>8</v>
-      </c>
-      <c r="S7" s="31" t="n">
-        <v>8</v>
-      </c>
-      <c r="T7" s="31" t="n">
-        <v>8</v>
-      </c>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
       <c r="U7" s="31"/>
       <c r="V7" s="31"/>
-      <c r="W7" s="31" t="n">
-        <v>8</v>
-      </c>
-      <c r="X7" s="31" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y7" s="31" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z7" s="31" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA7" s="31" t="n">
-        <v>8</v>
-      </c>
+      <c r="W7" s="31"/>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="31"/>
+      <c r="AA7" s="31"/>
       <c r="AB7" s="31"/>
       <c r="AC7" s="31"/>
-      <c r="AD7" s="31" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE7" s="31" t="n">
-        <v>8</v>
-      </c>
+      <c r="AD7" s="31"/>
+      <c r="AE7" s="31"/>
       <c r="AF7" s="82" t="n">
         <v>8</v>
       </c>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="AH7" s="34" t="s">
         <v>14</v>
@@ -12918,15 +13041,15 @@
       </c>
       <c r="R9" s="39" t="n">
         <f aca="false">SUM(R7:R8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="S9" s="39" t="n">
         <f aca="false">SUM(S7:S8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T9" s="39" t="n">
         <f aca="false">SUM(T7:T8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U9" s="39" t="n">
         <f aca="false">SUM(U7:U8)</f>
@@ -12938,23 +13061,23 @@
       </c>
       <c r="W9" s="39" t="n">
         <f aca="false">SUM(W7:W8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="X9" s="39" t="n">
         <f aca="false">SUM(X7:X8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y9" s="39" t="n">
         <f aca="false">SUM(Y7:Y8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="39" t="n">
         <f aca="false">SUM(Z7:Z8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AA9" s="39" t="n">
         <f aca="false">SUM(AA7:AA8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AB9" s="39" t="n">
         <f aca="false">SUM(AB7:AB8)</f>
@@ -12966,11 +13089,11 @@
       </c>
       <c r="AD9" s="39" t="n">
         <f aca="false">SUM(AD7:AD8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE9" s="39" t="n">
         <f aca="false">SUM(AE7:AE8)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AF9" s="39" t="n">
         <f aca="false">SUM(AF7:AF8)</f>
@@ -12978,7 +13101,7 @@
       </c>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -13292,24 +13415,44 @@
       <c r="O15" s="31"/>
       <c r="P15" s="31"/>
       <c r="Q15" s="31"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="31"/>
+      <c r="R15" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="S15" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="T15" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="U15" s="31"/>
       <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="31"/>
-      <c r="Y15" s="31"/>
-      <c r="Z15" s="31"/>
-      <c r="AA15" s="31"/>
+      <c r="W15" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="X15" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y15" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z15" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA15" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AB15" s="31"/>
       <c r="AC15" s="31"/>
-      <c r="AD15" s="31"/>
-      <c r="AE15" s="31"/>
+      <c r="AD15" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE15" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AF15" s="82"/>
       <c r="AG15" s="43" t="n">
         <f aca="false">SUM(B15:AF15)</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="AH15" s="34"/>
     </row>
@@ -13467,15 +13610,15 @@
       </c>
       <c r="R18" s="47" t="n">
         <f aca="false">SUM(R15:R17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S18" s="47" t="n">
         <f aca="false">SUM(S15:S17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T18" s="47" t="n">
         <f aca="false">SUM(T15:T17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U18" s="47" t="n">
         <f aca="false">SUM(U15:U17)</f>
@@ -13487,23 +13630,23 @@
       </c>
       <c r="W18" s="47" t="n">
         <f aca="false">SUM(W15:W17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X18" s="47" t="n">
         <f aca="false">SUM(X15:X17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y18" s="47" t="n">
         <f aca="false">SUM(Y15:Y17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z18" s="47" t="n">
         <f aca="false">SUM(Z15:Z17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA18" s="47" t="n">
         <f aca="false">SUM(AA15:AA17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB18" s="47" t="n">
         <f aca="false">SUM(AB15:AB17)</f>
@@ -13515,11 +13658,11 @@
       </c>
       <c r="AD18" s="47" t="n">
         <f aca="false">SUM(AD15:AD17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE18" s="47" t="n">
         <f aca="false">SUM(AE15:AE17)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF18" s="47" t="n">
         <f aca="false">SUM(AF15:AF17)</f>
@@ -13527,7 +13670,7 @@
       </c>
       <c r="AG18" s="48" t="n">
         <f aca="false">SUM(B18:AF18)</f>
-        <v>8</v>
+        <v>88</v>
       </c>
       <c r="AH18" s="49"/>
     </row>
@@ -13601,15 +13744,15 @@
       </c>
       <c r="R19" s="52" t="n">
         <f aca="false">R9+R13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="S19" s="52" t="n">
         <f aca="false">S9+S13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="T19" s="52" t="n">
         <f aca="false">T9+T13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U19" s="52" t="n">
         <f aca="false">U9+U13</f>
@@ -13621,23 +13764,23 @@
       </c>
       <c r="W19" s="52" t="n">
         <f aca="false">W9+W13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="X19" s="52" t="n">
         <f aca="false">X9+X13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="52" t="n">
         <f aca="false">Y9+Y13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="52" t="n">
         <f aca="false">Z9+Z13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AA19" s="52" t="n">
         <f aca="false">AA9+AA13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AB19" s="52" t="n">
         <f aca="false">AB9+AB13</f>
@@ -13649,11 +13792,11 @@
       </c>
       <c r="AD19" s="52" t="n">
         <f aca="false">AD9+AD13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE19" s="52" t="n">
         <f aca="false">AE9+AE13</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AF19" s="52" t="n">
         <f aca="false">AF9+AF13</f>
@@ -13661,7 +13804,7 @@
       </c>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="AH19" s="54"/>
     </row>
@@ -14288,7 +14431,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="AH8" activeCellId="0" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14693,42 +14836,84 @@
       <c r="A7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="C7" s="30"/>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
       <c r="F7" s="30"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="G7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="H7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="I7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="K7" s="30"/>
       <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
+      <c r="M7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="N7" s="76" t="n">
+        <v>8</v>
+      </c>
+      <c r="O7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="P7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="R7" s="31"/>
       <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
+      <c r="T7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="U7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="V7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="W7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="X7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="Y7" s="31"/>
       <c r="Z7" s="31"/>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="76"/>
+      <c r="AA7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="76" t="n">
+        <v>8</v>
+      </c>
       <c r="AF7" s="32"/>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34"/>
+        <v>160</v>
+      </c>
+      <c r="AH7" s="83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
@@ -14776,7 +14961,7 @@
       </c>
       <c r="B9" s="39" t="n">
         <f aca="false">SUM(B7:B8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="38" t="n">
         <f aca="false">SUM(C7:C8)</f>
@@ -14796,19 +14981,19 @@
       </c>
       <c r="G9" s="39" t="n">
         <f aca="false">SUM(G7:G8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H9" s="39" t="n">
         <f aca="false">SUM(H7:H8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9" s="39" t="n">
         <f aca="false">SUM(I7:I8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="39" t="n">
         <f aca="false">SUM(J7:J8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K9" s="38" t="n">
         <f aca="false">SUM(K7:K8)</f>
@@ -14820,23 +15005,23 @@
       </c>
       <c r="M9" s="39" t="n">
         <f aca="false">SUM(M7:M8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N9" s="77" t="n">
         <f aca="false">SUM(N7:N8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O9" s="39" t="n">
         <f aca="false">SUM(O7:O8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P9" s="39" t="n">
         <f aca="false">SUM(P7:P8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="39" t="n">
         <f aca="false">SUM(Q7:Q8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R9" s="39" t="n">
         <f aca="false">SUM(R7:R8)</f>
@@ -14848,23 +15033,23 @@
       </c>
       <c r="T9" s="39" t="n">
         <f aca="false">SUM(T7:T8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U9" s="39" t="n">
         <f aca="false">SUM(U7:U8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V9" s="39" t="n">
         <f aca="false">SUM(V7:V8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W9" s="39" t="n">
         <f aca="false">SUM(W7:W8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X9" s="39" t="n">
         <f aca="false">SUM(X7:X8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y9" s="39" t="n">
         <f aca="false">SUM(Y7:Y8)</f>
@@ -14876,28 +15061,28 @@
       </c>
       <c r="AA9" s="39" t="n">
         <f aca="false">SUM(AA7:AA8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB9" s="39" t="n">
         <f aca="false">SUM(AB7:AB8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC9" s="39" t="n">
         <f aca="false">SUM(AC7:AC8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD9" s="39" t="n">
         <f aca="false">SUM(AD7:AD8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE9" s="77" t="n">
         <f aca="false">SUM(AE7:AE8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF9" s="39"/>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -15448,7 +15633,7 @@
       </c>
       <c r="B19" s="52" t="n">
         <f aca="false">B9+B13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="51" t="n">
         <f aca="false">C9+C13</f>
@@ -15468,19 +15653,19 @@
       </c>
       <c r="G19" s="52" t="n">
         <f aca="false">G9+G13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H19" s="52" t="n">
         <f aca="false">H9+H13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I19" s="52" t="n">
         <f aca="false">I9+I13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J19" s="52" t="n">
         <f aca="false">J9+J13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K19" s="51" t="n">
         <f aca="false">K9+K13</f>
@@ -15492,23 +15677,23 @@
       </c>
       <c r="M19" s="52" t="n">
         <f aca="false">M9+M13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N19" s="79" t="n">
         <f aca="false">N9+N13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O19" s="52" t="n">
         <f aca="false">O9+O13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P19" s="52" t="n">
         <f aca="false">P9+P13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="52" t="n">
         <f aca="false">Q9+Q13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R19" s="52" t="n">
         <f aca="false">R9+R13</f>
@@ -15520,23 +15705,23 @@
       </c>
       <c r="T19" s="52" t="n">
         <f aca="false">T9+T13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U19" s="52" t="n">
         <f aca="false">U9+U13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V19" s="52" t="n">
         <f aca="false">V9+V13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W19" s="52" t="n">
         <f aca="false">W9+W13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X19" s="52" t="n">
         <f aca="false">X9+X13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y19" s="52" t="n">
         <f aca="false">Y9+Y13</f>
@@ -15548,28 +15733,28 @@
       </c>
       <c r="AA19" s="52" t="n">
         <f aca="false">AA9+AA13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB19" s="52" t="n">
         <f aca="false">AB9+AB13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC19" s="52" t="n">
         <f aca="false">AC9+AC13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD19" s="52" t="n">
         <f aca="false">AD9+AD13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE19" s="79" t="n">
         <f aca="false">AE9+AE13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF19" s="52"/>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="AH19" s="54"/>
     </row>
@@ -15610,7 +15795,7 @@
       <c r="AF20" s="56"/>
       <c r="AG20" s="57" t="n">
         <f aca="false">AG18+AG19</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="AH20" s="58"/>
     </row>
@@ -16196,7 +16381,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="AH7" activeCellId="0" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16244,11 +16429,11 @@
       <c r="U1" s="3"/>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
-      <c r="X1" s="83" t="n">
+      <c r="X1" s="84" t="n">
         <f aca="false">'Please complete'!C14</f>
         <v>39</v>
       </c>
-      <c r="Y1" s="83"/>
+      <c r="Y1" s="84"/>
       <c r="Z1" s="3" t="s">
         <v>2</v>
       </c>
@@ -16607,40 +16792,80 @@
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
+      <c r="D7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="H7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="I7" s="31"/>
       <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
+      <c r="K7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="L7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="M7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="N7" s="30"/>
-      <c r="O7" s="31"/>
+      <c r="O7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="P7" s="31"/>
       <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="76"/>
+      <c r="R7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="S7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="T7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="U7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="V7" s="76" t="n">
+        <v>8</v>
+      </c>
       <c r="W7" s="31"/>
       <c r="X7" s="31"/>
       <c r="Y7" s="30"/>
-      <c r="Z7" s="76"/>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
+      <c r="Z7" s="76" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AD7" s="31"/>
       <c r="AE7" s="30"/>
-      <c r="AF7" s="32"/>
+      <c r="AF7" s="32" t="n">
+        <v>8</v>
+      </c>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34"/>
+        <v>152</v>
+      </c>
+      <c r="AH7" s="83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
@@ -16696,23 +16921,23 @@
       </c>
       <c r="D9" s="39" t="n">
         <f aca="false">SUM(D7:D8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="39" t="n">
         <f aca="false">SUM(E7:E8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F9" s="39" t="n">
         <f aca="false">SUM(F7:F8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9" s="39" t="n">
         <f aca="false">SUM(G7:G8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H9" s="39" t="n">
         <f aca="false">SUM(H7:H8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9" s="39" t="n">
         <f aca="false">SUM(I7:I8)</f>
@@ -16724,15 +16949,15 @@
       </c>
       <c r="K9" s="39" t="n">
         <f aca="false">SUM(K7:K8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L9" s="39" t="n">
         <f aca="false">SUM(L7:L8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M9" s="39" t="n">
         <f aca="false">SUM(M7:M8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N9" s="38" t="n">
         <f aca="false">SUM(N7:N8)</f>
@@ -16740,7 +16965,7 @@
       </c>
       <c r="O9" s="39" t="n">
         <f aca="false">SUM(O7:O8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P9" s="39" t="n">
         <f aca="false">SUM(P7:P8)</f>
@@ -16752,23 +16977,23 @@
       </c>
       <c r="R9" s="39" t="n">
         <f aca="false">SUM(R7:R8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S9" s="39" t="n">
         <f aca="false">SUM(S7:S8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T9" s="39" t="n">
         <f aca="false">SUM(T7:T8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U9" s="39" t="n">
         <f aca="false">SUM(U7:U8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V9" s="77" t="n">
         <f aca="false">SUM(V7:V8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W9" s="39" t="n">
         <f aca="false">SUM(W7:W8)</f>
@@ -16784,19 +17009,19 @@
       </c>
       <c r="Z9" s="77" t="n">
         <f aca="false">SUM(Z7:Z8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA9" s="39" t="n">
         <f aca="false">SUM(AA7:AA8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB9" s="39" t="n">
         <f aca="false">SUM(AB7:AB8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC9" s="39" t="n">
         <f aca="false">SUM(AC7:AC8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD9" s="39" t="n">
         <f aca="false">SUM(AD7:AD8)</f>
@@ -16808,11 +17033,11 @@
       </c>
       <c r="AF9" s="39" t="n">
         <f aca="false">SUM(AF7:AF8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -17377,23 +17602,23 @@
       </c>
       <c r="D19" s="52" t="n">
         <f aca="false">D9+D13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E19" s="52" t="n">
         <f aca="false">E9+E13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F19" s="52" t="n">
         <f aca="false">F9+F13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G19" s="52" t="n">
         <f aca="false">G9+G13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H19" s="52" t="n">
         <f aca="false">H9+H13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I19" s="52" t="n">
         <f aca="false">I9+I13</f>
@@ -17405,15 +17630,15 @@
       </c>
       <c r="K19" s="52" t="n">
         <f aca="false">K9+K13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L19" s="52" t="n">
         <f aca="false">L9+L13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M19" s="52" t="n">
         <f aca="false">M9+M13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N19" s="51" t="n">
         <f aca="false">N9+N13</f>
@@ -17421,7 +17646,7 @@
       </c>
       <c r="O19" s="52" t="n">
         <f aca="false">O9+O13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P19" s="52" t="n">
         <f aca="false">P9+P13</f>
@@ -17433,23 +17658,23 @@
       </c>
       <c r="R19" s="52" t="n">
         <f aca="false">R9+R13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S19" s="52" t="n">
         <f aca="false">S9+S13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T19" s="52" t="n">
         <f aca="false">T9+T13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U19" s="52" t="n">
         <f aca="false">U9+U13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V19" s="79" t="n">
         <f aca="false">V9+V13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W19" s="52" t="n">
         <f aca="false">W9+W13</f>
@@ -17465,19 +17690,19 @@
       </c>
       <c r="Z19" s="79" t="n">
         <f aca="false">Z9+Z13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA19" s="52" t="n">
         <f aca="false">AA9+AA13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB19" s="52" t="n">
         <f aca="false">AB9+AB13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC19" s="52" t="n">
         <f aca="false">AC9+AC13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD19" s="52" t="n">
         <f aca="false">AD9+AD13</f>
@@ -17489,11 +17714,11 @@
       </c>
       <c r="AF19" s="52" t="n">
         <f aca="false">AF9+AF13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="AH19" s="54"/>
     </row>
@@ -17534,7 +17759,7 @@
       <c r="AF20" s="56"/>
       <c r="AG20" s="57" t="n">
         <f aca="false">AG18+AG19</f>
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="AH20" s="58"/>
     </row>
@@ -18120,7 +18345,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="AH7" activeCellId="0" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18525,42 +18750,88 @@
       <c r="A7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="B7" s="76" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" s="76" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="F7" s="31"/>
       <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+      <c r="H7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="I7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="L7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="M7" s="31"/>
       <c r="N7" s="31"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="31"/>
+      <c r="O7" s="76" t="n">
+        <v>8</v>
+      </c>
+      <c r="P7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="76" t="n">
+        <v>8</v>
+      </c>
+      <c r="S7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="T7" s="31"/>
       <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="31"/>
-      <c r="Z7" s="31"/>
+      <c r="V7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="W7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="X7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AA7" s="31"/>
       <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="31"/>
+      <c r="AC7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AF7" s="32"/>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34"/>
+        <v>176</v>
+      </c>
+      <c r="AH7" s="83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
@@ -18608,19 +18879,19 @@
       </c>
       <c r="B9" s="77" t="n">
         <f aca="false">SUM(B7:B8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="77" t="n">
         <f aca="false">SUM(C7:C8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9" s="39" t="n">
         <f aca="false">SUM(D7:D8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="39" t="n">
         <f aca="false">SUM(E7:E8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F9" s="39" t="n">
         <f aca="false">SUM(F7:F8)</f>
@@ -18632,23 +18903,23 @@
       </c>
       <c r="H9" s="39" t="n">
         <f aca="false">SUM(H7:H8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9" s="39" t="n">
         <f aca="false">SUM(I7:I8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="39" t="n">
         <f aca="false">SUM(J7:J8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K9" s="39" t="n">
         <f aca="false">SUM(K7:K8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L9" s="39" t="n">
         <f aca="false">SUM(L7:L8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M9" s="39" t="n">
         <f aca="false">SUM(M7:M8)</f>
@@ -18660,23 +18931,23 @@
       </c>
       <c r="O9" s="77" t="n">
         <f aca="false">SUM(O7:O8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P9" s="39" t="n">
         <f aca="false">SUM(P7:P8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="39" t="n">
         <f aca="false">SUM(Q7:Q8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R9" s="77" t="n">
         <f aca="false">SUM(R7:R8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S9" s="39" t="n">
         <f aca="false">SUM(S7:S8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T9" s="39" t="n">
         <f aca="false">SUM(T7:T8)</f>
@@ -18688,23 +18959,23 @@
       </c>
       <c r="V9" s="39" t="n">
         <f aca="false">SUM(V7:V8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W9" s="39" t="n">
         <f aca="false">SUM(W7:W8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X9" s="39" t="n">
         <f aca="false">SUM(X7:X8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y9" s="39" t="n">
         <f aca="false">SUM(Y7:Y8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z9" s="39" t="n">
         <f aca="false">SUM(Z7:Z8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA9" s="39" t="n">
         <f aca="false">SUM(AA7:AA8)</f>
@@ -18716,20 +18987,20 @@
       </c>
       <c r="AC9" s="39" t="n">
         <f aca="false">SUM(AC7:AC8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD9" s="39" t="n">
         <f aca="false">SUM(AD7:AD8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE9" s="39" t="n">
         <f aca="false">SUM(AE7:AE8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF9" s="39"/>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -19280,19 +19551,19 @@
       </c>
       <c r="B19" s="79" t="n">
         <f aca="false">B9+B13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="79" t="n">
         <f aca="false">C9+C13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D19" s="52" t="n">
         <f aca="false">D9+D13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E19" s="52" t="n">
         <f aca="false">E9+E13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F19" s="52" t="n">
         <f aca="false">F9+F13</f>
@@ -19304,23 +19575,23 @@
       </c>
       <c r="H19" s="52" t="n">
         <f aca="false">H9+H13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I19" s="52" t="n">
         <f aca="false">I9+I13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J19" s="52" t="n">
         <f aca="false">J9+J13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K19" s="52" t="n">
         <f aca="false">K9+K13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L19" s="52" t="n">
         <f aca="false">L9+L13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M19" s="52" t="n">
         <f aca="false">M9+M13</f>
@@ -19332,23 +19603,23 @@
       </c>
       <c r="O19" s="79" t="n">
         <f aca="false">O9+O13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P19" s="52" t="n">
         <f aca="false">P9+P13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="52" t="n">
         <f aca="false">Q9+Q13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R19" s="79" t="n">
         <f aca="false">R9+R13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S19" s="52" t="n">
         <f aca="false">S9+S13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T19" s="52" t="n">
         <f aca="false">T9+T13</f>
@@ -19360,23 +19631,23 @@
       </c>
       <c r="V19" s="52" t="n">
         <f aca="false">V9+V13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W19" s="52" t="n">
         <f aca="false">W9+W13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X19" s="52" t="n">
         <f aca="false">X9+X13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y19" s="52" t="n">
         <f aca="false">Y9+Y13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z19" s="52" t="n">
         <f aca="false">Z9+Z13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA19" s="52" t="n">
         <f aca="false">AA9+AA13</f>
@@ -19388,20 +19659,20 @@
       </c>
       <c r="AC19" s="52" t="n">
         <f aca="false">AC9+AC13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD19" s="52" t="n">
         <f aca="false">AD9+AD13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE19" s="52" t="n">
         <f aca="false">AE9+AE13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF19" s="52"/>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH19" s="54"/>
     </row>
@@ -19442,7 +19713,7 @@
       <c r="AF20" s="56"/>
       <c r="AG20" s="57" t="n">
         <f aca="false">AG18+AG19</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH20" s="58"/>
     </row>
@@ -20028,7 +20299,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="AH7" activeCellId="0" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20437,42 +20708,88 @@
       <c r="A7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="76" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="F7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="H7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="I7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
+      <c r="M7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="N7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="O7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="P7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="R7" s="31"/>
       <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
+      <c r="T7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="U7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="V7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="W7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="X7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="Y7" s="31"/>
       <c r="Z7" s="31"/>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="31"/>
+      <c r="AA7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AF7" s="32"/>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34"/>
+        <v>176</v>
+      </c>
+      <c r="AH7" s="83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
@@ -20520,11 +20837,11 @@
       </c>
       <c r="B9" s="77" t="n">
         <f aca="false">SUM(B7:B8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="39" t="n">
         <f aca="false">SUM(C7:C8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9" s="39" t="n">
         <f aca="false">SUM(D7:D8)</f>
@@ -20536,23 +20853,23 @@
       </c>
       <c r="F9" s="39" t="n">
         <f aca="false">SUM(F7:F8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9" s="39" t="n">
         <f aca="false">SUM(G7:G8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H9" s="39" t="n">
         <f aca="false">SUM(H7:H8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9" s="39" t="n">
         <f aca="false">SUM(I7:I8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="39" t="n">
         <f aca="false">SUM(J7:J8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K9" s="39" t="n">
         <f aca="false">SUM(K7:K8)</f>
@@ -20564,23 +20881,23 @@
       </c>
       <c r="M9" s="39" t="n">
         <f aca="false">SUM(M7:M8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N9" s="39" t="n">
         <f aca="false">SUM(N7:N8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O9" s="39" t="n">
         <f aca="false">SUM(O7:O8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P9" s="39" t="n">
         <f aca="false">SUM(P7:P8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="39" t="n">
         <f aca="false">SUM(Q7:Q8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R9" s="39" t="n">
         <f aca="false">SUM(R7:R8)</f>
@@ -20592,23 +20909,23 @@
       </c>
       <c r="T9" s="39" t="n">
         <f aca="false">SUM(T7:T8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U9" s="39" t="n">
         <f aca="false">SUM(U7:U8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V9" s="39" t="n">
         <f aca="false">SUM(V7:V8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W9" s="39" t="n">
         <f aca="false">SUM(W7:W8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X9" s="39" t="n">
         <f aca="false">SUM(X7:X8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y9" s="39" t="n">
         <f aca="false">SUM(Y7:Y8)</f>
@@ -20620,23 +20937,23 @@
       </c>
       <c r="AA9" s="39" t="n">
         <f aca="false">SUM(AA7:AA8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB9" s="39" t="n">
         <f aca="false">SUM(AB7:AB8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC9" s="39" t="n">
         <f aca="false">SUM(AC7:AC8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD9" s="39" t="n">
         <f aca="false">SUM(AD7:AD8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE9" s="39" t="n">
         <f aca="false">SUM(AE7:AE8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF9" s="39" t="n">
         <f aca="false">SUM(AF7:AF8)</f>
@@ -20644,7 +20961,7 @@
       </c>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -21201,11 +21518,11 @@
       </c>
       <c r="B19" s="79" t="n">
         <f aca="false">B9+B13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="52" t="n">
         <f aca="false">C9+C13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D19" s="52" t="n">
         <f aca="false">D9+D13</f>
@@ -21217,23 +21534,23 @@
       </c>
       <c r="F19" s="52" t="n">
         <f aca="false">F9+F13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G19" s="52" t="n">
         <f aca="false">G9+G13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H19" s="52" t="n">
         <f aca="false">H9+H13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I19" s="52" t="n">
         <f aca="false">I9+I13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J19" s="52" t="n">
         <f aca="false">J9+J13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K19" s="52" t="n">
         <f aca="false">K9+K13</f>
@@ -21245,23 +21562,23 @@
       </c>
       <c r="M19" s="52" t="n">
         <f aca="false">M9+M13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N19" s="52" t="n">
         <f aca="false">N9+N13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O19" s="52" t="n">
         <f aca="false">O9+O13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P19" s="52" t="n">
         <f aca="false">P9+P13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="52" t="n">
         <f aca="false">Q9+Q13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R19" s="52" t="n">
         <f aca="false">R9+R13</f>
@@ -21273,23 +21590,23 @@
       </c>
       <c r="T19" s="52" t="n">
         <f aca="false">T9+T13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U19" s="52" t="n">
         <f aca="false">U9+U13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V19" s="52" t="n">
         <f aca="false">V9+V13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W19" s="52" t="n">
         <f aca="false">W9+W13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X19" s="52" t="n">
         <f aca="false">X9+X13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y19" s="52" t="n">
         <f aca="false">Y9+Y13</f>
@@ -21301,23 +21618,23 @@
       </c>
       <c r="AA19" s="52" t="n">
         <f aca="false">AA9+AA13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB19" s="52" t="n">
         <f aca="false">AB9+AB13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC19" s="52" t="n">
         <f aca="false">AC9+AC13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD19" s="52" t="n">
         <f aca="false">AD9+AD13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE19" s="52" t="n">
         <f aca="false">AE9+AE13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF19" s="52" t="n">
         <f aca="false">AF9+AF13</f>
@@ -21325,7 +21642,7 @@
       </c>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH19" s="54"/>
     </row>
@@ -21366,7 +21683,7 @@
       <c r="AF20" s="56"/>
       <c r="AG20" s="57" t="n">
         <f aca="false">AG18+AG19</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH20" s="58"/>
     </row>
@@ -21951,7 +22268,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="AH7" activeCellId="0" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22361,41 +22678,87 @@
         <v>13</v>
       </c>
       <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="31"/>
+      <c r="C7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="76" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
+      <c r="J7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" s="76" t="n">
+        <v>8</v>
+      </c>
+      <c r="L7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="M7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="N7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
+      <c r="Q7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="S7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="T7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="U7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="V7" s="31"/>
       <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="31"/>
-      <c r="Z7" s="31"/>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
+      <c r="X7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AC7" s="31"/>
       <c r="AD7" s="31"/>
-      <c r="AE7" s="31"/>
-      <c r="AF7" s="31"/>
+      <c r="AE7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AF7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34"/>
+        <v>176</v>
+      </c>
+      <c r="AH7" s="83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
@@ -22447,23 +22810,23 @@
       </c>
       <c r="C9" s="39" t="n">
         <f aca="false">SUM(C7:C8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9" s="39" t="n">
         <f aca="false">SUM(D7:D8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="39" t="n">
         <f aca="false">SUM(E7:E8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F9" s="77" t="n">
         <f aca="false">SUM(F7:F8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9" s="39" t="n">
         <f aca="false">SUM(G7:G8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H9" s="39" t="n">
         <f aca="false">SUM(H7:H8)</f>
@@ -22475,23 +22838,23 @@
       </c>
       <c r="J9" s="39" t="n">
         <f aca="false">SUM(J7:J8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K9" s="77" t="n">
         <f aca="false">SUM(K7:K8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L9" s="39" t="n">
         <f aca="false">SUM(L7:L8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M9" s="39" t="n">
         <f aca="false">SUM(M7:M8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N9" s="39" t="n">
         <f aca="false">SUM(N7:N8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O9" s="39" t="n">
         <f aca="false">SUM(O7:O8)</f>
@@ -22503,23 +22866,23 @@
       </c>
       <c r="Q9" s="39" t="n">
         <f aca="false">SUM(Q7:Q8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R9" s="39" t="n">
         <f aca="false">SUM(R7:R8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S9" s="39" t="n">
         <f aca="false">SUM(S7:S8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T9" s="39" t="n">
         <f aca="false">SUM(T7:T8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U9" s="39" t="n">
         <f aca="false">SUM(U7:U8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V9" s="39" t="n">
         <f aca="false">SUM(V7:V8)</f>
@@ -22531,23 +22894,23 @@
       </c>
       <c r="X9" s="39" t="n">
         <f aca="false">SUM(X7:X8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y9" s="39" t="n">
         <f aca="false">SUM(Y7:Y8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z9" s="39" t="n">
         <f aca="false">SUM(Z7:Z8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA9" s="39" t="n">
         <f aca="false">SUM(AA7:AA8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB9" s="39" t="n">
         <f aca="false">SUM(AB7:AB8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC9" s="39" t="n">
         <f aca="false">SUM(AC7:AC8)</f>
@@ -22559,15 +22922,15 @@
       </c>
       <c r="AE9" s="39" t="n">
         <f aca="false">SUM(AE7:AE8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF9" s="39" t="n">
         <f aca="false">SUM(AF7:AF8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -23128,23 +23491,23 @@
       </c>
       <c r="C19" s="52" t="n">
         <f aca="false">C9+C13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D19" s="52" t="n">
         <f aca="false">D9+D13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E19" s="52" t="n">
         <f aca="false">E9+E13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F19" s="79" t="n">
         <f aca="false">F9+F13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G19" s="52" t="n">
         <f aca="false">G9+G13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H19" s="52" t="n">
         <f aca="false">H9+H13</f>
@@ -23156,23 +23519,23 @@
       </c>
       <c r="J19" s="52" t="n">
         <f aca="false">J9+J13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K19" s="79" t="n">
         <f aca="false">K9+K13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L19" s="52" t="n">
         <f aca="false">L9+L13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M19" s="52" t="n">
         <f aca="false">M9+M13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N19" s="52" t="n">
         <f aca="false">N9+N13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O19" s="52" t="n">
         <f aca="false">O9+O13</f>
@@ -23184,23 +23547,23 @@
       </c>
       <c r="Q19" s="52" t="n">
         <f aca="false">Q9+Q13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R19" s="52" t="n">
         <f aca="false">R9+R13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S19" s="52" t="n">
         <f aca="false">S9+S13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T19" s="52" t="n">
         <f aca="false">T9+T13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U19" s="52" t="n">
         <f aca="false">U9+U13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V19" s="52" t="n">
         <f aca="false">V9+V13</f>
@@ -23212,23 +23575,23 @@
       </c>
       <c r="X19" s="52" t="n">
         <f aca="false">X9+X13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y19" s="52" t="n">
         <f aca="false">Y9+Y13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z19" s="52" t="n">
         <f aca="false">Z9+Z13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AA19" s="52" t="n">
         <f aca="false">AA9+AA13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AB19" s="52" t="n">
         <f aca="false">AB9+AB13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC19" s="52" t="n">
         <f aca="false">AC9+AC13</f>
@@ -23240,15 +23603,15 @@
       </c>
       <c r="AE19" s="52" t="n">
         <f aca="false">AE9+AE13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF19" s="52" t="n">
         <f aca="false">AF9+AF13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH19" s="54"/>
     </row>
@@ -23289,7 +23652,7 @@
       <c r="AF20" s="56"/>
       <c r="AG20" s="57" t="n">
         <f aca="false">AG18+AG19</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH20" s="58"/>
     </row>
@@ -23875,7 +24238,7 @@
   <dimension ref="A1:AK34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="AH7" activeCellId="0" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24280,42 +24643,88 @@
       <c r="A7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
+      <c r="B7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
+      <c r="G7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="H7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="I7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="L7" s="31"/>
       <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
+      <c r="N7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="O7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="P7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="R7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="S7" s="31"/>
       <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="31"/>
+      <c r="U7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="V7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="W7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="X7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="Z7" s="31"/>
       <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="31"/>
+      <c r="AB7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD7" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE7" s="31" t="n">
+        <v>8</v>
+      </c>
       <c r="AF7" s="32"/>
       <c r="AG7" s="33" t="n">
         <f aca="false">SUM(B7:AF7)</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="34"/>
+        <v>176</v>
+      </c>
+      <c r="AH7" s="83" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="35"/>
@@ -24363,15 +24772,15 @@
       </c>
       <c r="B9" s="39" t="n">
         <f aca="false">SUM(B7:B8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C9" s="39" t="n">
         <f aca="false">SUM(C7:C8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9" s="39" t="n">
         <f aca="false">SUM(D7:D8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="39" t="n">
         <f aca="false">SUM(E7:E8)</f>
@@ -24383,23 +24792,23 @@
       </c>
       <c r="G9" s="39" t="n">
         <f aca="false">SUM(G7:G8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H9" s="39" t="n">
         <f aca="false">SUM(H7:H8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9" s="39" t="n">
         <f aca="false">SUM(I7:I8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="39" t="n">
         <f aca="false">SUM(J7:J8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K9" s="39" t="n">
         <f aca="false">SUM(K7:K8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L9" s="39" t="n">
         <f aca="false">SUM(L7:L8)</f>
@@ -24411,23 +24820,23 @@
       </c>
       <c r="N9" s="39" t="n">
         <f aca="false">SUM(N7:N8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O9" s="39" t="n">
         <f aca="false">SUM(O7:O8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P9" s="39" t="n">
         <f aca="false">SUM(P7:P8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="39" t="n">
         <f aca="false">SUM(Q7:Q8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R9" s="39" t="n">
         <f aca="false">SUM(R7:R8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S9" s="39" t="n">
         <f aca="false">SUM(S7:S8)</f>
@@ -24439,23 +24848,23 @@
       </c>
       <c r="U9" s="39" t="n">
         <f aca="false">SUM(U7:U8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V9" s="39" t="n">
         <f aca="false">SUM(V7:V8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W9" s="39" t="n">
         <f aca="false">SUM(W7:W8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X9" s="39" t="n">
         <f aca="false">SUM(X7:X8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y9" s="39" t="n">
         <f aca="false">SUM(Y7:Y8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z9" s="39" t="n">
         <f aca="false">SUM(Z7:Z8)</f>
@@ -24467,24 +24876,24 @@
       </c>
       <c r="AB9" s="39" t="n">
         <f aca="false">SUM(AB7:AB8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC9" s="39" t="n">
         <f aca="false">SUM(AC7:AC8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD9" s="39" t="n">
         <f aca="false">SUM(AD7:AD8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE9" s="39" t="n">
         <f aca="false">SUM(AE7:AE8)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF9" s="39"/>
       <c r="AG9" s="40" t="n">
         <f aca="false">SUM(B9:AF9)</f>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="AH9" s="34"/>
     </row>
@@ -25027,7 +25436,7 @@
         <f aca="false">SUM(B18:AF18)</f>
         <v>0</v>
       </c>
-      <c r="AH18" s="84"/>
+      <c r="AH18" s="85"/>
     </row>
     <row r="19" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="50" t="s">
@@ -25035,15 +25444,15 @@
       </c>
       <c r="B19" s="52" t="n">
         <f aca="false">B9+B13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C19" s="52" t="n">
         <f aca="false">C9+C13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D19" s="52" t="n">
         <f aca="false">D9+D13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E19" s="52" t="n">
         <f aca="false">E9+E13</f>
@@ -25055,23 +25464,23 @@
       </c>
       <c r="G19" s="52" t="n">
         <f aca="false">G9+G13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H19" s="52" t="n">
         <f aca="false">H9+H13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I19" s="52" t="n">
         <f aca="false">I9+I13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J19" s="52" t="n">
         <f aca="false">J9+J13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K19" s="52" t="n">
         <f aca="false">K9+K13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L19" s="52" t="n">
         <f aca="false">L9+L13</f>
@@ -25083,23 +25492,23 @@
       </c>
       <c r="N19" s="52" t="n">
         <f aca="false">N9+N13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O19" s="52" t="n">
         <f aca="false">O9+O13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P19" s="52" t="n">
         <f aca="false">P9+P13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="52" t="n">
         <f aca="false">Q9+Q13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R19" s="52" t="n">
         <f aca="false">R9+R13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S19" s="52" t="n">
         <f aca="false">S9+S13</f>
@@ -25111,23 +25520,23 @@
       </c>
       <c r="U19" s="52" t="n">
         <f aca="false">U9+U13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V19" s="52" t="n">
         <f aca="false">V9+V13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W19" s="52" t="n">
         <f aca="false">W9+W13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X19" s="52" t="n">
         <f aca="false">X9+X13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y19" s="52" t="n">
         <f aca="false">Y9+Y13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z19" s="52" t="n">
         <f aca="false">Z9+Z13</f>
@@ -25139,26 +25548,26 @@
       </c>
       <c r="AB19" s="52" t="n">
         <f aca="false">AB9+AB13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AC19" s="52" t="n">
         <f aca="false">AC9+AC13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AD19" s="52" t="n">
         <f aca="false">AD9+AD13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AE19" s="52" t="n">
         <f aca="false">AE9+AE13</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AF19" s="52"/>
       <c r="AG19" s="53" t="n">
         <f aca="false">SUM(B19:AF19)</f>
-        <v>0</v>
-      </c>
-      <c r="AH19" s="85"/>
+        <v>176</v>
+      </c>
+      <c r="AH19" s="86"/>
     </row>
     <row r="20" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="55" t="s">
@@ -25197,9 +25606,9 @@
       <c r="AF20" s="56"/>
       <c r="AG20" s="57" t="n">
         <f aca="false">AG18+AG19</f>
-        <v>0</v>
-      </c>
-      <c r="AH20" s="86"/>
+        <v>176</v>
+      </c>
+      <c r="AH20" s="87"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="59"/>

</xml_diff>